<commit_message>
Ignore temporary Excel files
</commit_message>
<xml_diff>
--- a/Excel/data.xlsx
+++ b/Excel/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PeteL\eclipse-workspace\DataDrivenTesting.Npru\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A3C5623-586E-41AB-854D-57C2138F0278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98066627-F8D6-4D97-BADA-F1093492786B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A5955695-74A6-425B-B12D-E25843C6EFE5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="63">
   <si>
     <t>ธนวัฒน์</t>
   </si>
@@ -141,23 +141,97 @@
   </si>
   <si>
     <t>70000</t>
+  </si>
+  <si>
+    <t>TC02</t>
+  </si>
+  <si>
+    <t>นาง</t>
+  </si>
+  <si>
+    <t>ณัฐ์สุดา</t>
+  </si>
+  <si>
+    <t>รงทอง</t>
+  </si>
+  <si>
+    <t>Ms.</t>
+  </si>
+  <si>
+    <t>Natsuda</t>
+  </si>
+  <si>
+    <t>Rongthong</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>1849100011356</t>
+  </si>
+  <si>
+    <t>Nan_0006</t>
+  </si>
+  <si>
+    <t>664259006@webmail.npru.ac.th</t>
+  </si>
+  <si>
+    <t>56</t>
+  </si>
+  <si>
+    <t>สุราษฐานี</t>
+  </si>
+  <si>
+    <t>ชัยยา</t>
+  </si>
+  <si>
+    <t>ทุ้ง</t>
+  </si>
+  <si>
+    <t>84110</t>
+  </si>
+  <si>
+    <t>ทดสอบ</t>
+  </si>
+  <si>
+    <t>สามารถ</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Skill</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2004</t>
+  </si>
+  <si>
+    <t>17357542276667</t>
+  </si>
+  <si>
+    <t>P24567861</t>
+  </si>
+  <si>
+    <t>0Test0@webmail.npru.ac.th</t>
+  </si>
+  <si>
+    <t>141</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -221,49 +295,35 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="3" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="5">
-    <cellStyle name="Currency" xfId="1" builtinId="4"/>
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
-    <cellStyle name="Hyperlink 2" xfId="4" xr:uid="{5CE2A51B-75EA-454B-AB57-4555DB6A897C}"/>
+  <cellStyles count="4">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink 2" xfId="3" xr:uid="{5CE2A51B-75EA-454B-AB57-4555DB6A897C}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="3" xr:uid="{338B182F-7169-4D45-AFD4-C1ADD0C30784}"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{338B182F-7169-4D45-AFD4-C1ADD0C30784}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -598,7 +658,7 @@
   <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -617,145 +677,248 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="23.4" x14ac:dyDescent="0.6">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="N1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="O1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="P1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="Q1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="R1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="S1" s="9" t="s">
+      <c r="S1" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="J2" s="10">
+      <c r="J2" s="6">
         <v>2004</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="K2" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="6">
+      <c r="M2" s="2">
         <v>8555640258</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="N2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="O2" s="10" t="s">
+      <c r="O2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="P2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="Q2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="R2" s="6" t="s">
+      <c r="R2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="S2" s="10" t="s">
+      <c r="S2" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="3"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
+    <row r="3" spans="1:19" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="A3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="J3" s="6">
+        <v>2004</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="M3" s="2">
+        <v>9824222972</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S3" s="6" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="I4" s="4"/>
-      <c r="J4" s="1"/>
+    <row r="4" spans="1:19" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="A4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="M4" s="2">
+        <v>1166648656</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="O4" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="S4" s="6" t="s">
+        <v>34</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="N2" r:id="rId1" xr:uid="{F058DA2F-35BD-4A3E-96A0-DF6E3F77108D}"/>
+    <hyperlink ref="N3" r:id="rId2" xr:uid="{127A1F5B-9B0C-4B34-B32D-321EAD439DE5}"/>
+    <hyperlink ref="N4" r:id="rId3" xr:uid="{8FCFBF06-A267-4733-9F1F-1A200EDFBBC5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>